<commit_message>
optimised NSGA-2 implementation and evaluation in python with multithreading and parallel computing, monitoring and logging.
</commit_message>
<xml_diff>
--- a/output/allocation_summary_nsga_610.xlsx
+++ b/output/allocation_summary_nsga_610.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E22"/>
+  <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -462,13 +462,13 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="B2" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C2" t="n">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="D2" t="inlineStr">
         <is>
@@ -477,13 +477,13 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>26</t>
+          <t>25</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B3" t="n">
         <v>3</v>
@@ -493,18 +493,18 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>5,6</t>
+          <t>5,8</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>19,18</t>
+          <t>19,19</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="B4" t="n">
         <v>3</v>
@@ -514,12 +514,12 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>15,21</t>
+          <t>6,15,21</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>26,24</t>
+          <t>18,24,2</t>
         </is>
       </c>
     </row>
@@ -535,33 +535,33 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>8,14</t>
+          <t>14,21</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>20,30</t>
+          <t>28,22</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>50</v>
+        <v>57</v>
       </c>
       <c r="B6" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C6" t="n">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>2,7</t>
+          <t>2</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>25,14</t>
+          <t>26</t>
         </is>
       </c>
     </row>
@@ -582,19 +582,19 @@
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>26,24</t>
+          <t>27,23</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>90</v>
+        <v>74</v>
       </c>
       <c r="B8" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C8" t="n">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="D8" t="inlineStr">
         <is>
@@ -603,7 +603,7 @@
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>24,16</t>
+          <t>28,22</t>
         </is>
       </c>
     </row>
@@ -624,19 +624,19 @@
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>34,14,1</t>
+          <t>36,12,2</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>247</v>
+        <v>240</v>
       </c>
       <c r="B10" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C10" t="n">
-        <v>30</v>
+        <v>50</v>
       </c>
       <c r="D10" t="inlineStr">
         <is>
@@ -645,13 +645,13 @@
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>3,27</t>
+          <t>4,46</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>280</v>
+        <v>248</v>
       </c>
       <c r="B11" t="n">
         <v>2</v>
@@ -661,81 +661,81 @@
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>12,18</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>1,19</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>292</v>
+        <v>257</v>
       </c>
       <c r="B12" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C12" t="n">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>9,11</t>
+          <t>7,9</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>30,10</t>
+          <t>3,27</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>385</v>
+        <v>314</v>
       </c>
       <c r="B13" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C13" t="n">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>9</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>16</t>
+          <t>3</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>406</v>
+        <v>378</v>
       </c>
       <c r="B14" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C14" t="n">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>17</t>
+          <t>11,16</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>36</t>
+          <t>24,26</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>414</v>
+        <v>442</v>
       </c>
       <c r="B15" t="n">
         <v>3</v>
@@ -745,33 +745,33 @@
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>18</t>
+          <t>17</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>19</t>
+          <t>35</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>455</v>
+        <v>470</v>
       </c>
       <c r="B16" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C16" t="n">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>16</t>
+          <t>27</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>26</t>
+          <t>47</t>
         </is>
       </c>
     </row>
@@ -780,46 +780,46 @@
         <v>478</v>
       </c>
       <c r="B17" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C17" t="n">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>19</t>
+          <t>19,25,26</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>36</t>
+          <t>35,2,7</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="n">
-        <v>493</v>
+        <v>482</v>
       </c>
       <c r="B18" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C18" t="n">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>27</t>
+          <t>16</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>48</t>
+          <t>1</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="n">
-        <v>519</v>
+        <v>509</v>
       </c>
       <c r="B19" t="n">
         <v>3</v>
@@ -829,12 +829,12 @@
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>23</t>
+          <t>23,24</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>20</t>
+          <t>18,11</t>
         </is>
       </c>
     </row>
@@ -850,54 +850,33 @@
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>22</t>
+          <t>22,24</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>19</t>
+          <t>18,22</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="n">
-        <v>567</v>
+        <v>580</v>
       </c>
       <c r="B21" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C21" t="n">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>25,26</t>
+          <t>25</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>38,8</t>
-        </is>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" t="n">
-        <v>595</v>
-      </c>
-      <c r="B22" t="n">
-        <v>1</v>
-      </c>
-      <c r="C22" t="n">
-        <v>30</v>
-      </c>
-      <c r="D22" t="inlineStr">
-        <is>
-          <t>24</t>
-        </is>
-      </c>
-      <c r="E22" t="inlineStr">
-        <is>
-          <t>30</t>
+          <t>40</t>
         </is>
       </c>
     </row>

</xml_diff>